<commit_message>
actualización de documentos y backend login, registro
</commit_message>
<xml_diff>
--- a/Desarrollo/Edutec/Gestión/Sprint Backlog.xlsx
+++ b/Desarrollo/Edutec/Gestión/Sprint Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6D180C-2712-4298-AA80-B14E3BCF2CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC0C161-7EB2-4399-AD8E-404D04877599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,17 @@
     <sheet name="Hoja3" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Hoja 1" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miVOqr7TWK4pZoKsQco/LoFvR8/ew=="/>
     </ext>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="126">
   <si>
     <t>Universidad Nacional Mayor de San Marcos</t>
   </si>
@@ -384,9 +393,6 @@
     <t>Tarea 5 (T01-T5)</t>
   </si>
   <si>
-    <t>Tarea 7 (C01-T7)</t>
-  </si>
-  <si>
     <t>Tarea 6 (C01-T6)</t>
   </si>
   <si>
@@ -406,6 +412,9 @@
   </si>
   <si>
     <t>Tarea 6 (C02-T6)</t>
+  </si>
+  <si>
+    <t>Tarea 7 (C02-T7)</t>
   </si>
 </sst>
 </file>
@@ -793,7 +802,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1042,13 +1051,19 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1058,12 +1073,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1073,6 +1082,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1290,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1624,17 +1636,17 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A11" s="98" t="s">
+      <c r="A11" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="100"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="92"/>
       <c r="J11" s="3"/>
       <c r="K11" s="12"/>
       <c r="L11" s="3"/>
@@ -1670,16 +1682,16 @@
         <v>23</v>
       </c>
       <c r="F12" s="17">
+        <v>44509</v>
+      </c>
+      <c r="G12" s="17">
         <v>44510</v>
-      </c>
-      <c r="G12" s="17">
-        <v>44511</v>
       </c>
       <c r="H12" s="18">
         <v>4</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -1703,29 +1715,29 @@
       <c r="A13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>23</v>
+      <c r="D13" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>27</v>
       </c>
       <c r="F13" s="17">
         <v>44510</v>
       </c>
       <c r="G13" s="17">
-        <v>44519</v>
-      </c>
-      <c r="H13" s="18">
-        <v>16</v>
+        <v>44511</v>
+      </c>
+      <c r="H13" s="14">
+        <v>4</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1745,97 +1757,97 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
+    <row r="14" spans="1:26" ht="17.25" customHeight="1">
       <c r="A14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="21" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="17">
-        <v>44510</v>
+        <v>44511</v>
       </c>
       <c r="G14" s="17">
-        <v>44511</v>
-      </c>
-      <c r="H14" s="14">
-        <v>4</v>
+        <v>44515</v>
+      </c>
+      <c r="H14" s="21">
+        <v>8</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+      <c r="Z14" s="22"/>
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1">
       <c r="A15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="15" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>27</v>
       </c>
       <c r="F15" s="17">
-        <v>44511</v>
+        <v>44515</v>
       </c>
       <c r="G15" s="17">
-        <v>44515</v>
-      </c>
-      <c r="H15" s="21">
-        <v>8</v>
+        <v>44516</v>
+      </c>
+      <c r="H15" s="15">
+        <v>4</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
-      <c r="T15" s="22"/>
-      <c r="U15" s="22"/>
-      <c r="V15" s="22"/>
-      <c r="W15" s="22"/>
-      <c r="X15" s="22"/>
-      <c r="Y15" s="22"/>
-      <c r="Z15" s="22"/>
+        <v>82</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1">
       <c r="A16" s="13" t="s">
@@ -1848,22 +1860,22 @@
         <v>33</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="17">
-        <v>44515</v>
+        <v>44516</v>
       </c>
       <c r="G16" s="17">
-        <v>44516</v>
+        <v>44517</v>
       </c>
       <c r="H16" s="15">
         <v>4</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -1887,32 +1899,32 @@
       <c r="A17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="17">
-        <v>44516</v>
+        <v>44518</v>
       </c>
       <c r="G17" s="17">
-        <v>44517</v>
+        <v>44519</v>
       </c>
       <c r="H17" s="15">
         <v>4</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+      <c r="K17" s="23"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -1930,35 +1942,35 @@
       <c r="Z17" s="3"/>
     </row>
     <row r="18" spans="1:26" ht="17.25" customHeight="1">
-      <c r="A18" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="17">
-        <v>44518</v>
-      </c>
-      <c r="G18" s="17">
-        <v>44519</v>
-      </c>
-      <c r="H18" s="15">
+      <c r="C18" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="28">
+        <v>44510</v>
+      </c>
+      <c r="G18" s="28">
+        <v>44511</v>
+      </c>
+      <c r="H18" s="26">
         <v>4</v>
       </c>
-      <c r="I18" s="19" t="s">
-        <v>123</v>
+      <c r="I18" s="29" t="s">
+        <v>82</v>
       </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="23"/>
+      <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -1983,25 +1995,25 @@
         <v>20</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E19" s="27" t="s">
         <v>37</v>
       </c>
       <c r="F19" s="28">
-        <v>44510</v>
+        <v>44511</v>
       </c>
       <c r="G19" s="28">
-        <v>44511</v>
+        <v>44515</v>
       </c>
       <c r="H19" s="26">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="I19" s="29" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -2029,25 +2041,25 @@
         <v>20</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E20" s="27" t="s">
         <v>37</v>
       </c>
       <c r="F20" s="28">
-        <v>44511</v>
+        <v>44515</v>
       </c>
       <c r="G20" s="28">
-        <v>44515</v>
+        <v>44516</v>
       </c>
       <c r="H20" s="26">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -2075,25 +2087,25 @@
         <v>20</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E21" s="27" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="28">
-        <v>44515</v>
+        <v>44516</v>
       </c>
       <c r="G21" s="28">
-        <v>44516</v>
+        <v>44518</v>
       </c>
       <c r="H21" s="26">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I21" s="29" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -2113,36 +2125,36 @@
       <c r="Y21" s="3"/>
       <c r="Z21" s="3"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
       <c r="A22" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="30" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E22" s="27" t="s">
         <v>37</v>
       </c>
       <c r="F22" s="28">
-        <v>44516</v>
+        <v>44518</v>
       </c>
       <c r="G22" s="28">
-        <v>44518</v>
-      </c>
-      <c r="H22" s="26">
-        <v>8</v>
+        <v>44519</v>
+      </c>
+      <c r="H22" s="30">
+        <v>4</v>
       </c>
       <c r="I22" s="29" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="K22" s="23"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -2159,36 +2171,36 @@
       <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1">
-      <c r="A23" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="30" t="s">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
+      <c r="A23" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="28">
-        <v>44518</v>
-      </c>
-      <c r="G23" s="28">
+      <c r="C23" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="36">
+        <v>44510</v>
+      </c>
+      <c r="G23" s="36">
         <v>44519</v>
       </c>
-      <c r="H23" s="30">
-        <v>4</v>
-      </c>
-      <c r="I23" s="29" t="s">
-        <v>123</v>
+      <c r="H23" s="37">
+        <v>16</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>82</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="23"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -2206,16 +2218,14 @@
       <c r="Z23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A24" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="32" t="s">
+      <c r="A24" s="107"/>
+      <c r="B24" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="34" t="s">
+      <c r="C24" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="35" t="s">
@@ -2231,7 +2241,7 @@
         <v>8</v>
       </c>
       <c r="I24" s="38" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -2259,10 +2269,10 @@
         <v>20</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>43</v>
@@ -2277,7 +2287,7 @@
         <v>8</v>
       </c>
       <c r="I25" s="38" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -2305,7 +2315,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D26" s="34" t="s">
         <v>29</v>
@@ -2351,7 +2361,7 @@
         <v>20</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="D27" s="34" t="s">
         <v>31</v>
@@ -2397,7 +2407,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D28" s="34" t="s">
         <v>32</v>
@@ -2507,7 +2517,7 @@
         <v>8</v>
       </c>
       <c r="I30" s="47" t="s">
-        <v>24</v>
+        <v>122</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -2673,7 +2683,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D34" s="44" t="s">
         <v>34</v>
@@ -2826,11 +2836,11 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A39" s="92" t="s">
+      <c r="A39" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="93"/>
-      <c r="C39" s="93"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="98"/>
       <c r="D39" s="94"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -2856,7 +2866,7 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A40" s="101" t="s">
+      <c r="A40" s="93" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="94"/>
@@ -2890,10 +2900,10 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="91"/>
+      <c r="B41" s="96"/>
       <c r="C41" s="60" t="s">
         <v>19</v>
       </c>
@@ -2924,10 +2934,10 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A42" s="90" t="s">
+      <c r="A42" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="91"/>
+      <c r="B42" s="96"/>
       <c r="C42" s="60" t="s">
         <v>35</v>
       </c>
@@ -2958,10 +2968,10 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A43" s="90" t="s">
+      <c r="A43" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="91"/>
+      <c r="B43" s="96"/>
       <c r="C43" s="60" t="s">
         <v>41</v>
       </c>
@@ -2992,10 +3002,10 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="91"/>
+      <c r="B44" s="96"/>
       <c r="C44" s="60" t="s">
         <v>47</v>
       </c>
@@ -3088,10 +3098,10 @@
       <c r="B47" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="95" t="s">
+      <c r="C47" s="99" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="95"/>
+      <c r="D47" s="99"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -3117,15 +3127,15 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="88">
-        <v>44509</v>
+        <v>44508</v>
       </c>
       <c r="B48" s="89">
         <v>1</v>
       </c>
-      <c r="C48" s="96" t="s">
+      <c r="C48" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="D48" s="97"/>
+      <c r="D48" s="101"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -3156,10 +3166,10 @@
       <c r="B49" s="89">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C49" s="96" t="s">
+      <c r="C49" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="97"/>
+      <c r="D49" s="101"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -29953,16 +29963,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -31211,14 +31221,14 @@
       <c r="A11" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="100"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="91"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="92"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1">
@@ -31416,14 +31426,14 @@
       <c r="A18" s="103" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="99"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="100"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
+      <c r="G18" s="91"/>
+      <c r="H18" s="91"/>
+      <c r="I18" s="92"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1">
       <c r="A19" s="79" t="s">
@@ -31647,13 +31657,13 @@
         <v>54</v>
       </c>
       <c r="B28" s="105"/>
-      <c r="C28" s="91"/>
+      <c r="C28" s="96"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="A29" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="91"/>
+      <c r="B29" s="96"/>
       <c r="C29" s="58" t="s">
         <v>56</v>
       </c>
@@ -31665,7 +31675,7 @@
       <c r="A30" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="91"/>
+      <c r="B30" s="96"/>
       <c r="C30" s="83" t="s">
         <v>35</v>
       </c>
@@ -31677,7 +31687,7 @@
       <c r="A31" s="102" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="91"/>
+      <c r="B31" s="96"/>
       <c r="C31" s="83" t="s">
         <v>63</v>
       </c>
@@ -31689,7 +31699,7 @@
       <c r="A32" s="102" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="91"/>
+      <c r="B32" s="96"/>
       <c r="C32" s="83" t="s">
         <v>73</v>
       </c>
@@ -31701,7 +31711,7 @@
       <c r="A33" s="102" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="91"/>
+      <c r="B33" s="96"/>
       <c r="C33" s="83" t="s">
         <v>69</v>
       </c>
@@ -31713,7 +31723,7 @@
       <c r="A34" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="91"/>
+      <c r="B34" s="96"/>
       <c r="C34" s="83" t="s">
         <v>71</v>
       </c>
@@ -31725,7 +31735,7 @@
       <c r="A35" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="91"/>
+      <c r="B35" s="96"/>
       <c r="C35" s="83" t="s">
         <v>66</v>
       </c>

</xml_diff>